<commit_message>
Successfully generated new dataframe using list comprehension with the creation of a new dictionary, which is then used to create a new dataframe
Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,661 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A2:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 5 5600 </t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-5-5600-ryzen-5-5000-series/p/N82E16819113736</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$199.00 –</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 5 5600 </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-5-5600-ryzen-5-5000-series/p/N82E16819113736</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$199.00 (7 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Intel Core i9</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i9-12900k-core-i9-12th-gen/p/N82E16819118339</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$609.99 (18 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 5 5600X </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-5-5600x/p/N82E16819113666</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$219.99 (18 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-12600k-core-i5-12th-gen/p/N82E16819118347</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$277.98 (19 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 7 5700X </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-7-5700x-ryzen-7-5000-series/p/N82E16819113735</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$298.99 (8 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i7-12700k-core-i7-12th-gen/p/N82E16819118343</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$449.99 (20 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 5 5600G </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-5-5600g-ryzen-5-5000-g-series/p/N82E16819113683</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$209.98 (17 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Intel Core i9</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i9-12900ks-core-i9-12th-gen/p/N82E16819118392</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$779.98 (9 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 7 5800X </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-7-5800x/p/N82E16819113665</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$323.99 (16 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Intel Core i3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i3-10100f-core-i3-10th-gen/p/N82E16819118223</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$84.99 (17 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 5 3rd Gen </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-5-3600/p/N82E16819113569</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$209.99 (13 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-12400f-core-i5-12th-gen/p/N82E16819118358</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$169.99 (17 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 9 5900X </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-9-5900x/p/N82E16819113664</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$399.99 (14 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-12400f-core-i5-12th-gen/p/N82E16819118360</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$159.99 (15 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 7 5700G </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-7-5700g-ryzen-7-5000-g-series/p/N82E16819113682</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$278.99 (16 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i7-11700kf-core-i7-11th-gen/p/N82E16819118260</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$298.99 (13 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Intel Core i3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i3-12100f-core-i3-12th-gen/p/N82E16819118357</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$99.99 (16 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 5 5500 </t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-5-5500-ryzen-5-5000-series/p/N82E16819113737</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$159.00 (4 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i7-12700kf-core-i7-12th-gen/p/N82E16819118345</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$364.99 (21 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Intel Core i9</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i9-11900k-core-i9-11th-gen/p/N82E16819118231</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$397.97 (19 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-12600kf-core-i5-12th-gen/p/N82E16819118349</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$260.98 (13 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMD Ryzen 9 5950X </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/amd-ryzen-9-5950x/p/N82E16819113663</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$559.98 (12 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-11600k-core-i5-11th-gen/p/N82E16819118235</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$210.99 (22 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i7-12700f-core-i7-12th-gen/p/N82E16819118359</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$312.96 (12 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Intel Core i3</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i3-10105-core-i3-10th-gen/p/N82E16819118248</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$112.83 (24 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Intel Core i9</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i9-12900kf-core-i9-12th-gen/p/N82E16819118341</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$549.99 (13 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i7-10700f-core-i7-10th-gen/p/N82E16819118131</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$249.99 (21 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-11500-core-i5-11th-gen/p/N82E16819118240</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$197.19 (14 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-12500-core-i5-12th-gen/p/N82E16819118374</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$202.98 (14 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Intel Core i7</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i7-11700k-core-i7-11th-gen/p/N82E16819118233</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$317.99 (19 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Intel Core i9</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i9-11900f-core-i9-11th-gen/p/N82E16819118262</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>$379.99 (12 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Intel Core i7 10th Gen </t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i7-10700k-core-i7-10th-gen/p/N82E16819118123</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>$328.97 (19 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-11400-core-i5-11th-gen/p/N82E16819118241</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>$156.56 (28 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-10600k-core-i5-10th-gen/p/N82E16819118124</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>$212.97 (15 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Intel Core i5</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i5-11600-core-i5-11th-gen/p/N82E16819118238</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>$216.41 (13 Offers)–</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Intel Core i9</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://www.newegg.com/intel-core-i9-10900kf-core-i9-10th-gen/p/N82E16819118127</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>$346.99 (17 Offers)–</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all remaining get_functions. Now adds all of that data to a dataframe. (Vulnerable to changes to websites HTML - needs error catching). Prints all data to a csv.
Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -827,102 +827,102 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 9 5950X </t>
+          <t>Intel Core i5</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/amd-ryzen-9-5950x/p/N82E16819113663</t>
+          <t>https://www.newegg.com/intel-core-i5-11600k-core-i5-11th-gen/p/N82E16819118235</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>$559.98 (12 Offers)–</t>
+          <t>$210.99 (22 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel Core i7</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-11600k-core-i5-11th-gen/p/N82E16819118235</t>
+          <t>https://www.newegg.com/intel-core-i7-12700f-core-i7-12th-gen/p/N82E16819118359</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>$210.99 (22 Offers)–</t>
+          <t>$312.96 (12 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>Intel Core i3</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-12700f-core-i7-12th-gen/p/N82E16819118359</t>
+          <t>https://www.newegg.com/intel-core-i3-10105-core-i3-10th-gen/p/N82E16819118248</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>$312.96 (12 Offers)–</t>
+          <t>$112.83 (24 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Intel Core i3</t>
+          <t>Intel Core i9</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i3-10105-core-i3-10th-gen/p/N82E16819118248</t>
+          <t>https://www.newegg.com/intel-core-i9-12900kf-core-i9-12th-gen/p/N82E16819118341</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>$112.83 (24 Offers)–</t>
+          <t>$549.99 (13 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t>Intel Core i7</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i9-12900kf-core-i9-12th-gen/p/N82E16819118341</t>
+          <t>https://www.newegg.com/intel-core-i7-10700f-core-i7-10th-gen/p/N82E16819118131</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>$549.99 (13 Offers)–</t>
+          <t>$249.99 (21 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>Intel Core i5</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-10700f-core-i7-10th-gen/p/N82E16819118131</t>
+          <t>https://www.newegg.com/intel-core-i5-11500-core-i5-11th-gen/p/N82E16819118240</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>$249.99 (21 Offers)–</t>
+          <t>$197.19 (14 Offers)–</t>
         </is>
       </c>
     </row>
@@ -934,80 +934,80 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-11500-core-i5-11th-gen/p/N82E16819118240</t>
+          <t>https://www.newegg.com/intel-core-i5-12500-core-i5-12th-gen/p/N82E16819118374</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>$197.19 (14 Offers)–</t>
+          <t>$202.98 (14 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel Core i7</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-12500-core-i5-12th-gen/p/N82E16819118374</t>
+          <t>https://www.newegg.com/intel-core-i7-11700k-core-i7-11th-gen/p/N82E16819118233</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>$202.98 (14 Offers)–</t>
+          <t>$317.99 (19 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>Intel Core i9</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-11700k-core-i7-11th-gen/p/N82E16819118233</t>
+          <t>https://www.newegg.com/intel-core-i9-11900f-core-i9-11th-gen/p/N82E16819118262</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>$317.99 (19 Offers)–</t>
+          <t>$379.99 (12 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t xml:space="preserve">Intel Core i7 10th Gen </t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i9-11900f-core-i9-11th-gen/p/N82E16819118262</t>
+          <t>https://www.newegg.com/intel-core-i7-10700k-core-i7-10th-gen/p/N82E16819118123</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>$379.99 (12 Offers)–</t>
+          <t>$328.97 (19 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intel Core i7 10th Gen </t>
+          <t>Intel Core i5</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-10700k-core-i7-10th-gen/p/N82E16819118123</t>
+          <t>https://www.newegg.com/intel-core-i5-11400-core-i5-11th-gen/p/N82E16819118241</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>$328.97 (19 Offers)–</t>
+          <t>$156.56 (28 Offers)–</t>
         </is>
       </c>
     </row>
@@ -1019,12 +1019,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-11400-core-i5-11th-gen/p/N82E16819118241</t>
+          <t>https://www.newegg.com/intel-core-i5-10600k-core-i5-10th-gen/p/N82E16819118124</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>$156.56 (28 Offers)–</t>
+          <t>$212.97 (15 Offers)–</t>
         </is>
       </c>
     </row>
@@ -1036,46 +1036,46 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-10600k-core-i5-10th-gen/p/N82E16819118124</t>
+          <t>https://www.newegg.com/intel-core-i5-11600-core-i5-11th-gen/p/N82E16819118238</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>$212.97 (15 Offers)–</t>
+          <t>$216.41 (13 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel Core i9</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-11600-core-i5-11th-gen/p/N82E16819118238</t>
+          <t>https://www.newegg.com/intel-core-i9-10900kf-core-i9-10th-gen/p/N82E16819118127</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>$216.41 (13 Offers)–</t>
+          <t>$346.99 (17 Offers)–</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t xml:space="preserve">AMD Ryzen 9 5950X </t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i9-10900kf-core-i9-10th-gen/p/N82E16819118127</t>
+          <t>https://www.newegg.com/amd-ryzen-9-5950x/p/N82E16819113663</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>$346.99 (17 Offers)–</t>
+          <t>$559.98 (12 Offers)–</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Now successfully inserts new column data into dataframe with WebFunctions. WebFunctions needs to be updated to pull correct data.
Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C39"/>
+  <dimension ref="A2:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,646 +436,1406 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
+          <t>Brand</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Price</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Socket</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Cores</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Threads </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 5 5600 </t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Ryzen 5 5600</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/amd-ryzen-5-5600-ryzen-5-5000-series/p/N82E16819113736</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>$199.00 –</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 5 5600 </t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Ryzen 5 5600</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/amd-ryzen-5-5600-ryzen-5-5000-series/p/N82E16819113736</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>$199.00 (7 Offers)–</t>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$199.00 (8 Offers)–</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Core i9-12900K</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/intel-core-i9-12900k-core-i9-12th-gen/p/N82E16819118339</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>$609.99 (18 Offers)–</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>16-Core (8P+8E)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>24</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 5 5600X </t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Ryzen 5 5600X</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/amd-ryzen-5-5600x/p/N82E16819113666</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>$219.99 (18 Offers)–</t>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$208.99 (17 Offers)–</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Core i5-12600K</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/intel-core-i5-12600k-core-i5-12th-gen/p/N82E16819118347</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>$277.98 (19 Offers)–</t>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$277.98 (18 Offers)–</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>10-Core (6P+4E)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 7 5700X </t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Ryzen 7 5700X</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/amd-ryzen-7-5700x-ryzen-7-5000-series/p/N82E16819113735</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>$298.99 (8 Offers)–</t>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$283.99 (8 Offers)–</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>4.6 GHz</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Core i7-12700K</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/intel-core-i7-12700k-core-i7-12th-gen/p/N82E16819118343</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>$449.99 (20 Offers)–</t>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$376.99 (20 Offers)–</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>12-Core (8P+4E)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>20</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 5 5600G </t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Ryzen 5 5600G</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/amd-ryzen-5-5600g-ryzen-5-5000-g-series/p/N82E16819113683</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>$209.98 (17 Offers)–</t>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$178.98 (17 Offers)–</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Core i9-12900KS</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>https://www.newegg.com/intel-core-i9-12900ks-core-i9-12th-gen/p/N82E16819118392</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>$779.98 (9 Offers)–</t>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$779.99 (10 Offers)–</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>16-Core (8P+8E)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>24</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 7 5800X </t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/amd-ryzen-7-5800x/p/N82E16819113665</t>
+          <t>Ryzen 7 5800X3D</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$323.99 (16 Offers)–</t>
+          <t>https://www.newegg.com/amd-ryzen-7-5800x3d-ryzen-7-5000-series/p/N82E16819113734</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$449.00 (6 Offers)–</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>3.4 GHz</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Intel Core i3</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i3-10100f-core-i3-10th-gen/p/N82E16819118223</t>
+          <t>Ryzen 7 5800X</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$84.99 (17 Offers)–</t>
+          <t>https://www.newegg.com/amd-ryzen-7-5800x/p/N82E16819113665</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$329.00 (15 Offers)–</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 5 3rd Gen </t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/amd-ryzen-5-3600/p/N82E16819113569</t>
+          <t>Core i3-10100F</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$209.99 (13 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i3-10100f-core-i3-10th-gen/p/N82E16819118223</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$79.98 (20 Offers)–</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Quad-Core</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-12400f-core-i5-12th-gen/p/N82E16819118358</t>
+          <t>Ryzen 5 3600</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$169.99 (17 Offers)–</t>
+          <t>https://www.newegg.com/amd-ryzen-5-3600/p/N82E16819113569</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$188.88 (14 Offers)–</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 9 5900X </t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/amd-ryzen-9-5900x/p/N82E16819113664</t>
+          <t>Core i5-12400</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$399.99 (14 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-12400f-core-i5-12th-gen/p/N82E16819118358</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$169.99 (18 Offers)–</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-12400f-core-i5-12th-gen/p/N82E16819118360</t>
+          <t>Ryzen 9 5900X</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$159.99 (15 Offers)–</t>
+          <t>https://www.newegg.com/amd-ryzen-9-5900x/p/N82E16819113664</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$399.99 (14 Offers)–</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>12-Core</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>24</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 7 5700G </t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/amd-ryzen-7-5700g-ryzen-7-5000-g-series/p/N82E16819113682</t>
+          <t>Core i5-12400F</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>$278.99 (16 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-12400f-core-i5-12th-gen/p/N82E16819118360</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$159.99 (16 Offers)–</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-11700kf-core-i7-11th-gen/p/N82E16819118260</t>
+          <t>Ryzen 7 5700G</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$298.99 (13 Offers)–</t>
+          <t>https://www.newegg.com/amd-ryzen-7-5700g-ryzen-7-5000-g-series/p/N82E16819113682</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>$278.99 (17 Offers)–</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Intel Core i3</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i3-12100f-core-i3-12th-gen/p/N82E16819118357</t>
+          <t>Core i7-11700KF</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$99.99 (16 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i7-11700kf-core-i7-11th-gen/p/N82E16819118260</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>$298.99 (14 Offers)–</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 5 5500 </t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/amd-ryzen-5-5500-ryzen-5-5000-series/p/N82E16819113737</t>
+          <t>Core i3-12100F</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$159.00 (4 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i3-12100f-core-i3-12th-gen/p/N82E16819118357</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>$107.99 (17 Offers)–</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Quad-Core</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-12700kf-core-i7-12th-gen/p/N82E16819118345</t>
+          <t>Ryzen 5 5500</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>$364.99 (21 Offers)–</t>
+          <t>https://www.newegg.com/amd-ryzen-5-5500-ryzen-5-5000-series/p/N82E16819113737</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>$139.00 (6 Offers)–</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>4.2 GHz</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i9-11900k-core-i9-11th-gen/p/N82E16819118231</t>
+          <t>Core i7-12700KF</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$397.97 (19 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i7-12700kf-core-i7-12th-gen/p/N82E16819118345</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>$364.99 (21 Offers)–</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>12-Core (8P+4E)</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>20</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-12600kf-core-i5-12th-gen/p/N82E16819118349</t>
+          <t>Core i9-11900K</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>$260.98 (13 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i9-11900k-core-i9-11th-gen/p/N82E16819118231</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>$397.97 (19 Offers)–</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-11600k-core-i5-11th-gen/p/N82E16819118235</t>
+          <t>Core i5-12600KF</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>$210.99 (22 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-12600kf-core-i5-12th-gen/p/N82E16819118349</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>$259.99 (13 Offers)–</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>10-Core (6P+4E)</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-12700f-core-i7-12th-gen/p/N82E16819118359</t>
+          <t>Ryzen 9 5950X</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>$312.96 (12 Offers)–</t>
+          <t>https://www.newegg.com/amd-ryzen-9-5950x/p/N82E16819113663</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>$599.99 (12 Offers)–</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>16-Core</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>32</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Intel Core i3</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i3-10105-core-i3-10th-gen/p/N82E16819118248</t>
+          <t>Core i5-11600K</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>$112.83 (24 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-11600k-core-i5-11th-gen/p/N82E16819118235</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>$210.99 (21 Offers)–</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i9-12900kf-core-i9-12th-gen/p/N82E16819118341</t>
+          <t>Core i7-12700F</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>$549.99 (13 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i7-12700f-core-i7-12th-gen/p/N82E16819118359</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>$312.96 (13 Offers)–</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>12-Core (8P+4E)</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>20</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-10700f-core-i7-10th-gen/p/N82E16819118131</t>
+          <t>Core i3-10105</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>$249.99 (21 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i3-10105-core-i3-10th-gen/p/N82E16819118248</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>$112.83 (24 Offers)–</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Quad-Core</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-11500-core-i5-11th-gen/p/N82E16819118240</t>
+          <t>Core i9-12900KF</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>$197.19 (14 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i9-12900kf-core-i9-12th-gen/p/N82E16819118341</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>$549.99 (13 Offers)–</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>16-Core (8P+8E)</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>24</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-12500-core-i5-12th-gen/p/N82E16819118374</t>
+          <t>Core i7-10700F</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>$202.98 (14 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i7-10700f-core-i7-10th-gen/p/N82E16819118131</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>$249.99 (20 Offers)–</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Intel Core i7</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-11700k-core-i7-11th-gen/p/N82E16819118233</t>
+          <t>Core i5-11500</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>$317.99 (19 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-11500-core-i5-11th-gen/p/N82E16819118240</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>$197.19 (13 Offers)–</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i9-11900f-core-i9-11th-gen/p/N82E16819118262</t>
+          <t>Core i5-12500</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>$379.99 (12 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-12500-core-i5-12th-gen/p/N82E16819118374</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>$202.98 (16 Offers)–</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Intel Core i7 10th Gen </t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i7-10700k-core-i7-10th-gen/p/N82E16819118123</t>
+          <t>Core i7-11700K</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>$328.97 (19 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i7-11700k-core-i7-11th-gen/p/N82E16819118233</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>$317.99 (17 Offers)–</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-11400-core-i5-11th-gen/p/N82E16819118241</t>
+          <t>Core i9-11900F</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>$156.56 (28 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i9-11900f-core-i9-11th-gen/p/N82E16819118262</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>$359.99 (13 Offers)–</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-10600k-core-i5-10th-gen/p/N82E16819118124</t>
+          <t>Core i7-10700K</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>$212.97 (15 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i7-10700k-core-i7-10th-gen/p/N82E16819118123</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>$328.97 (18 Offers)–</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Intel Core i5</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i5-11600-core-i5-11th-gen/p/N82E16819118238</t>
+          <t>Core i5-11400</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>$216.41 (13 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-11400-core-i5-11th-gen/p/N82E16819118241</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>$151.97 (31 Offers)–</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Intel Core i9</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/intel-core-i9-10900kf-core-i9-10th-gen/p/N82E16819118127</t>
+          <t>Core i5-10600K</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>$346.99 (17 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-10600k-core-i5-10th-gen/p/N82E16819118124</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>$211.97 (15 Offers)–</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMD Ryzen 9 5950X </t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.newegg.com/amd-ryzen-9-5950x/p/N82E16819113663</t>
+          <t>Core i5-11600</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>$559.98 (12 Offers)–</t>
+          <t>https://www.newegg.com/intel-core-i5-11600-core-i5-11th-gen/p/N82E16819118238</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>$216.41 (13 Offers)–</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Rewrote comments to update, need to include price.
Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Socket</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Cores</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Threads</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Operating Frequency</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Max Operating Frequency</t>
         </is>
@@ -483,25 +488,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>3.5 GHz</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>4.4 GHz</t>
         </is>
@@ -520,25 +530,30 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>3.5 GHz</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>4.4 GHz</t>
         </is>
@@ -557,25 +572,30 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>16-Core (8P+8E)</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>P-core Base Frequency: 3.2 GHzE-core Base Frequency: 2.4 GHz</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.2 GHzSingle P-core Turbo Frequency: Up to 5.1 GHzSingle E-core Turbo Frequency: Up to 3.9 GHz</t>
         </is>
@@ -594,25 +614,30 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>3.7 GHz</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>4.6 GHz</t>
         </is>
@@ -631,25 +656,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>12-Core (8P+4E)</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
@@ -668,25 +698,30 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>3.9 GHz</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>4.4 GHz</t>
         </is>
@@ -705,25 +740,30 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>10-Core (6P+4E)</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>P-core Base Frequency: 3.7 GHzE-core Base Frequency: 2.8 GHz</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Single P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.6 GHz</t>
         </is>
@@ -742,25 +782,30 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>8-Core</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>4.6 GHz</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>DNE</t>
         </is>
@@ -779,25 +824,30 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>16-Core (8P+8E)</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>P-core Base Frequency: 3.4 GHzE-core Base Frequency: 2.5 GHz</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Intel Thermal Velocity Boost Max Frequency: 5.5 GHzIntel Turbo Boost Max Technology 3.0 Frequency: 5.3 GHzPerformance-core Max Turbo Frequency: 5.2 GHzEfficient-core Max Turbo Frequency: 4 GHz</t>
         </is>
@@ -816,25 +866,30 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>8-Core</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>3.8 GHz</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>4.7 GHz</t>
         </is>
@@ -853,25 +908,30 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>8-Core</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>2.5 GHz</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>4.9 GHz</t>
         </is>
@@ -890,25 +950,30 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>3.6 GHz</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>4.2 GHz</t>
         </is>
@@ -927,25 +992,30 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>8-Core</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>3.5 GHz</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>Intel Thermal Velocity Boost Frequency: 5.30 GHzIntel Turbo Boost Max Technology 3.0 Frequency: 5.20 GHzIntel Turbo Boost Technology 2.0 Frequency: 5.10 GHz</t>
         </is>
@@ -964,25 +1034,30 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>8-Core</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>3.8 GHz</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>4.6 GHz</t>
         </is>
@@ -1001,25 +1076,30 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>12-Core (8P+4E)</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>P-core Base Frequency: 2.1 GHzE-core Base Frequency: 1.6 GHz</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 4.9 GHzP-core Turbo Frequency: Up to 4.8 GHzE-core Turbo Frequency: Up to 3.6 GHz</t>
         </is>
@@ -1038,25 +1118,30 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>4.2 GHz</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>DNE</t>
         </is>
@@ -1075,25 +1160,30 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>2.5 GHz</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>4.4 GHz</t>
         </is>
@@ -1112,25 +1202,30 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>12-Core</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>3.7 GHz</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>4.8 GHz</t>
         </is>
@@ -1149,25 +1244,30 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>2.9 GHz</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>4.30 GHz</t>
         </is>
@@ -1186,25 +1286,30 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>16-Core</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>32</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>3.4 GHz</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>4.9 GHz</t>
         </is>
@@ -1223,25 +1328,30 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>2.5 GHz</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>4.4 GHz</t>
         </is>
@@ -1260,25 +1370,30 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>10-Core (6P+4E)</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>P-core Base Frequency: 3.7 GHzE-core Base Frequency: 2.8 GHz</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>Single P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.6 GHz</t>
         </is>
@@ -1297,25 +1412,30 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>8-Core</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>2.9 GHz</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>4.80 GHz</t>
         </is>
@@ -1334,25 +1454,30 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>2.6 GHz</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>4.4 GHz</t>
         </is>
@@ -1371,25 +1496,30 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>Socket AM4</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>Quad-Core</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>3.6 GHz</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>Up to 3.9 GHz</t>
         </is>
@@ -1408,25 +1538,30 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>LGA 1700</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>16-Core (8P+8E)</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>P-core Base Frequency: 3.2 GHzE-core Base Frequency: 2.4 GHz</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.2 GHzSingle P-core Turbo Frequency: Up to 5.1 GHzSingle E-core Turbo Frequency: Up to 3.9 GHz</t>
         </is>
@@ -1445,25 +1580,30 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>8-Core</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>3.6 GHz</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>Intel Turbo Boost Max Technology 3.0 Frequency: 5.00 GHzIntel Turbo Boost Technology 2.0 Frequency: 4.90 GHz</t>
         </is>
@@ -1477,32 +1617,37 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Core i7-11700KF</t>
+          <t>Core i3-10100F</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>8-Core</t>
-        </is>
-      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>3.6 GHz</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>5.0 GHz</t>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>4.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1514,32 +1659,37 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Core i3-10100F</t>
+          <t>Core i3-12100F</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>Quad-Core</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>3.6 GHz</t>
-        </is>
-      </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>4.30 GHz</t>
+          <t>3.3 GHz</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>4.3 GHz</t>
         </is>
       </c>
     </row>
@@ -1551,32 +1701,37 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Core i3-12100F</t>
+          <t>Core i7-10700K</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>3.3 GHz</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>4.3 GHz</t>
+          <t>3.8 GHz</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>5.10 GHz</t>
         </is>
       </c>
     </row>
@@ -1588,32 +1743,37 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Core i7-10700K</t>
+          <t>Core i7-12700KF</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>12-Core (8P+4E)</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>5.10 GHz</t>
+          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
       </c>
     </row>
@@ -1625,32 +1785,37 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Core i7-12700KF</t>
+          <t>Core i5-10600K</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12-Core (8P+4E)</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
+          <t>4.1 GHz</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>4.80 GHz</t>
         </is>
       </c>
     </row>
@@ -1662,32 +1827,37 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Core i5-10600K</t>
+          <t>Core i5-11600KF</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>6-Core</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>4.1 GHz</t>
-        </is>
-      </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>4.80 GHz</t>
+          <t>3.9 GHz</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>4.9 GHz</t>
         </is>
       </c>
     </row>
@@ -1699,32 +1869,37 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Core i5-11600KF</t>
+          <t>Core i3-10105</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>6-Core</t>
-        </is>
-      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>3.9 GHz</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>4.9 GHz</t>
+          <t>3.7 GHz</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -1736,32 +1911,37 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Core i3-10105</t>
+          <t>Core i9-10900K</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Quad-Core</t>
-        </is>
-      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10-Core</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>3.7 GHz</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>4.4 GHz</t>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>5.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1773,32 +1953,37 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Core i9-10900K</t>
+          <t>Core i9-12900</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>10-Core</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>16-Core (8P+8E)</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>5.30 GHz</t>
+          <t>P-core Base Frequency: 2.4 GHzE-core Base Frequency: 1.8 GHz</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.1 GHzP-core Turbo Frequency: Up to 5.0 GHzE-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
       </c>
     </row>
@@ -1810,32 +1995,37 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Core i9-12900</t>
+          <t>Core i7-11700KF</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>16-Core (8P+8E)</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 2.4 GHzE-core Base Frequency: 1.8 GHz</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.1 GHzP-core Turbo Frequency: Up to 5.0 GHzE-core Turbo Frequency: Up to 3.8 GHz</t>
+          <t>3.6 GHz</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>5.0 GHz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated comments, fixed price being added incorrectly to Excel sheet
Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$199</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$199</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$598</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$206</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$399</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$179</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -740,7 +740,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$262</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$299</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$779</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$308</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -908,7 +908,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$313</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$164</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -992,7 +992,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$371</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$272</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$312</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$139</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$193</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$399</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$151</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$549</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$169</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$259</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$249</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$149</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$134</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$549</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$317</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1617,12 +1617,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Core i3-10100F</t>
+          <t>Core i7-11700KF</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$298</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1632,12 +1632,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>4.30 GHz</t>
+          <t>5.0 GHz</t>
         </is>
       </c>
     </row>
@@ -1659,17 +1659,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Core i3-12100F</t>
+          <t>Core i3-10100F</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$78</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1684,12 +1684,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>3.3 GHz</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>4.3 GHz</t>
+          <t>4.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1701,37 +1701,37 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Core i7-10700K</t>
+          <t>Core i3-12100F</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$107</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>3.3 GHz</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>5.10 GHz</t>
+          <t>4.3 GHz</t>
         </is>
       </c>
     </row>
@@ -1743,37 +1743,37 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Core i7-12700KF</t>
+          <t>Core i7-10700K</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$328</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>12-Core (8P+4E)</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
+          <t>3.8 GHz</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
+          <t>5.10 GHz</t>
         </is>
       </c>
     </row>
@@ -1785,37 +1785,37 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Core i5-10600K</t>
+          <t>Core i7-12700KF</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$363</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12-Core (8P+4E)</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>4.1 GHz</t>
+          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>4.80 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
       </c>
     </row>
@@ -1827,12 +1827,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Core i5-11600KF</t>
+          <t>Core i5-10600K</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$203</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1852,12 +1852,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>3.9 GHz</t>
+          <t>4.1 GHz</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>4.9 GHz</t>
+          <t>4.80 GHz</t>
         </is>
       </c>
     </row>
@@ -1869,12 +1869,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Core i3-10105</t>
+          <t>Core i5-11600KF</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$209</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1884,22 +1884,22 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>3.9 GHz</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>4.4 GHz</t>
+          <t>4.9 GHz</t>
         </is>
       </c>
     </row>
@@ -1911,12 +1911,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Core i9-10900K</t>
+          <t>Core i3-10105</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$111</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1926,12 +1926,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>10-Core</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>5.30 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -1953,37 +1953,37 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Core i9-12900</t>
+          <t>Core i9-10900K</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$389</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>16-Core (8P+8E)</t>
+          <t>10-Core</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 2.4 GHzE-core Base Frequency: 1.8 GHz</t>
+          <t>3.7 GHz</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.1 GHzP-core Turbo Frequency: Up to 5.0 GHzE-core Turbo Frequency: Up to 3.8 GHz</t>
+          <t>5.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1995,37 +1995,37 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Core i7-11700KF</t>
+          <t>Core i9-12900</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>['199', '199', '598', '206', '399', '179', '279', '299', '779', '308', '313', '164', '371', '272', '312', '139', '193', '399', '151', '549', '169', '259', '249', '149', '134', '549', '317', '78', '107', '328', '363', '203', '209', '111', '389', '508', '298']</t>
+          <t>$508</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16-Core (8P+8E)</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>P-core Base Frequency: 2.4 GHzE-core Base Frequency: 1.8 GHz</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>5.0 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.1 GHzP-core Turbo Frequency: Up to 5.0 GHzE-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Starting to switch pages, and creating the system that switched between computer components.
Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -530,7 +530,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$199</t>
+          <t>$129</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$598</t>
+          <t>$289</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$206</t>
+          <t>$224</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$399</t>
+          <t>$110</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$179</t>
+          <t>$199</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -740,7 +740,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$262</t>
+          <t>$360</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$299</t>
+          <t>$124</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$779</t>
+          <t>$339</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$308</t>
+          <t>$179</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -908,7 +908,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$313</t>
+          <t>$202</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$164</t>
+          <t>$268</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -992,7 +992,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$371</t>
+          <t>$214</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$272</t>
+          <t>$229</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$312</t>
+          <t>$78</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$139</t>
+          <t>$369</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>$193</t>
+          <t>$172</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$399</t>
+          <t>$199</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$151</t>
+          <t>$360</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$549</t>
+          <t>$469</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>$169</t>
+          <t>$119</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$259</t>
+          <t>$229</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>$249</t>
+          <t>$315</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>$149</t>
+          <t>$76</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>$134</t>
+          <t>$144</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>$549</t>
+          <t>$154</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>$317</t>
+          <t>$299</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>$298</t>
+          <t>$405</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>$78</t>
+          <t>$201</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>$107</t>
+          <t>$3,129</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>$328</t>
+          <t>$164</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1790,7 +1790,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>$363</t>
+          <t>$549</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>$203</t>
+          <t>$1,459</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1869,12 +1869,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Core i5-11600KF</t>
+          <t>Core i3-10105</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>$209</t>
+          <t>$59</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1884,22 +1884,22 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>3.9 GHz</t>
+          <t>3.7 GHz</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>4.9 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -1911,12 +1911,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Core i3-10105</t>
+          <t>Core i9-10900K</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>$111</t>
+          <t>$179</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1926,12 +1926,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>10-Core</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>4.4 GHz</t>
+          <t>5.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1953,37 +1953,37 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Core i9-10900K</t>
+          <t>Core i9-12900</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>$389</t>
+          <t>$359</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>10-Core</t>
+          <t>16-Core (8P+8E)</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>P-core Base Frequency: 2.4 GHzE-core Base Frequency: 1.8 GHz</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>5.30 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.1 GHzP-core Turbo Frequency: Up to 5.0 GHzE-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
       </c>
     </row>
@@ -1995,12 +1995,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Core i9-12900</t>
+          <t>Core i7-12700</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>$508</t>
+          <t>$354</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2010,22 +2010,22 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>16-Core (8P+8E)</t>
+          <t>12-Core (8P+4E)</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 2.4 GHzE-core Base Frequency: 1.8 GHz</t>
+          <t>P-core Base Frequency: 2.1 GHzE-core Base Frequency: 1.6 GHz</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.1 GHzP-core Turbo Frequency: Up to 5.0 GHzE-core Turbo Frequency: Up to 3.8 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 4.9 GHzP-core Turbo Frequency: Up to 4.8 GHzE-core Turbo Frequency: Up to 3.6 GHz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Program successfully navigates to different pages and pulls requested data.
Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -2,28 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -37,12 +41,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,14 +74,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -434,42 +456,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Socket</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Cores</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Threads</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Operating Frequency</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Max Operating Frequency</t>
         </is>
@@ -530,7 +552,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$129</t>
+          <t>$199</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -572,7 +594,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$289</t>
+          <t>$597</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -614,7 +636,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$224</t>
+          <t>$199</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -656,7 +678,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$110</t>
+          <t>$384</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -698,7 +720,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$199</t>
+          <t>$178</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -740,7 +762,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$360</t>
+          <t>$277</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -782,7 +804,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$124</t>
+          <t>$298</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -824,7 +846,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$339</t>
+          <t>$749</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -866,7 +888,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$179</t>
+          <t>$328</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -908,7 +930,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>$202</t>
+          <t>$313</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -950,7 +972,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$268</t>
+          <t>$164</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -992,7 +1014,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>$214</t>
+          <t>$393</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1034,7 +1056,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$229</t>
+          <t>$281</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1076,7 +1098,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$78</t>
+          <t>$312</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1118,7 +1140,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$369</t>
+          <t>$138</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1160,7 +1182,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>$172</t>
+          <t>$194</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1202,7 +1224,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$199</t>
+          <t>$399</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1244,7 +1266,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$360</t>
+          <t>$151</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1286,7 +1308,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$469</t>
+          <t>$549</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1328,7 +1350,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>$119</t>
+          <t>$169</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1370,7 +1392,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$229</t>
+          <t>$259</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1412,7 +1434,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>$315</t>
+          <t>$249</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1454,7 +1476,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>$76</t>
+          <t>$149</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1486,42 +1508,42 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Ryzen 3 3100</t>
+          <t>Core i9-12900KF</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>$144</t>
+          <t>$549</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>16-Core (8P+8E)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>P-core Base Frequency: 3.2 GHzE-core Base Frequency: 2.4 GHz</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Up to 3.9 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.2 GHzSingle P-core Turbo Frequency: Up to 5.1 GHzSingle E-core Turbo Frequency: Up to 3.9 GHz</t>
         </is>
       </c>
     </row>
@@ -1533,37 +1555,37 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Core i9-12900KF</t>
+          <t>Core i7-11700KF</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>$154</t>
+          <t>$298</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>16-Core (8P+8E)</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.2 GHzE-core Base Frequency: 2.4 GHz</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.2 GHzSingle P-core Turbo Frequency: Up to 5.1 GHzSingle E-core Turbo Frequency: Up to 3.9 GHz</t>
+          <t>5.0 GHz</t>
         </is>
       </c>
     </row>
@@ -1575,12 +1597,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Core i7-11700K</t>
+          <t>Core i3-10100F</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>$299</t>
+          <t>$78</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1590,12 +1612,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1605,7 +1627,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Intel Turbo Boost Max Technology 3.0 Frequency: 5.00 GHzIntel Turbo Boost Technology 2.0 Frequency: 4.90 GHz</t>
+          <t>4.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1617,37 +1639,37 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Core i7-11700KF</t>
+          <t>Core i3-12100F</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>$405</t>
+          <t>$107</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>3.3 GHz</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>5.0 GHz</t>
+          <t>4.3 GHz</t>
         </is>
       </c>
     </row>
@@ -1659,12 +1681,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Core i3-10100F</t>
+          <t>Core i7-10700K</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>$201</t>
+          <t>$328</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1674,22 +1696,22 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>3.8 GHz</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>4.30 GHz</t>
+          <t>5.10 GHz</t>
         </is>
       </c>
     </row>
@@ -1701,37 +1723,37 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Core i3-12100F</t>
+          <t>Core i5-11500</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>$3,129</t>
+          <t>$194</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>3.3 GHz</t>
+          <t>2.7 GHz</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>4.3 GHz</t>
+          <t>4.6 GHz</t>
         </is>
       </c>
     </row>
@@ -1743,37 +1765,37 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Core i7-10700K</t>
+          <t>Core i7-12700KF</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>$164</t>
+          <t>$363</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>12-Core (8P+4E)</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>5.10 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
       </c>
     </row>
@@ -1785,37 +1807,37 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Core i7-12700KF</t>
+          <t>Core i5-10600K</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>$549</t>
+          <t>$203</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>12-Core (8P+4E)</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
+          <t>4.1 GHz</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
+          <t>4.80 GHz</t>
         </is>
       </c>
     </row>
@@ -1827,12 +1849,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Core i5-10600K</t>
+          <t>Core i5-11600KF</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>$1,459</t>
+          <t>$209</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1852,12 +1874,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>4.1 GHz</t>
+          <t>3.9 GHz</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>4.80 GHz</t>
+          <t>4.9 GHz</t>
         </is>
       </c>
     </row>
@@ -1874,7 +1896,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>$59</t>
+          <t>$111</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1916,7 +1938,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>$179</t>
+          <t>$389</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1958,7 +1980,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>$359</t>
+          <t>$508</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2000,7 +2022,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>$354</t>
+          <t>$342</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">

</xml_diff>

<commit_message>
Fixed a couple problems, and figured out one more to get program fully operational. Need to catch ValueError in inputting data into DataFrame.
Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,7 +510,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$D</t>
+          <t>$199</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$N</t>
+          <t>$174</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$E</t>
+          <t>$559</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -620,6 +620,1434 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.2 GHzSingle P-core Turbo Frequency: Up to 5.1 GHzSingle E-core Turbo Frequency: Up to 3.9 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ryzen 5 5600X</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$174</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>3.7 GHz</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>4.6 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Core i7-11700K</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$317</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>3.6 GHz</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: 5.00 GHzIntel Turbo Boost Technology 2.0 Frequency: 4.90 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ryzen 7 5700X</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$272</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>4.6 GHz</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>DNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Core i5-12400F</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$154</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2.5 GHz</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>4.4 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ryzen 9 5900X</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$398</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12-Core</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>3.7 GHz</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>4.8 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Core i5-12600K</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$229</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>10-Core (6P+4E)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>P-core Base Frequency: 3.7 GHzE-core Base Frequency: 2.8 GHz</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Single P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.6 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ryzen 5 5500</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$139</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>4.2 GHz</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>DNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Core i9-11900K</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$364</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>3.5 GHz</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Intel Thermal Velocity Boost Frequency: 5.30 GHzIntel Turbo Boost Max Technology 3.0 Frequency: 5.20 GHzIntel Turbo Boost Technology 2.0 Frequency: 5.10 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Ryzen 7 5800X</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$274</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>3.8 GHz</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>4.7 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Core i7-12700K</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$349</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12-Core (8P+4E)</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ryzen 5 5600G</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$178</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>3.9 GHz</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>4.4 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Core i5-10400F</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$119</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2.9 GHz</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>4.30 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ryzen 5 3600</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$164</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>3.6 GHz</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>4.2 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Core i3-12100F</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$106</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Quad-Core</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>3.3 GHz</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>4.3 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Ryzen 9 5950X</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$553</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>16-Core</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>3.4 GHz</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>4.9 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Core i5-12400</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$193</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2.5 GHz</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>4.4 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ryzen 7 5700G</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$291</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>3.8 GHz</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>4.6 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Core i5-10600K</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$203</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>4.1 GHz</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>4.80 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ryzen 7 5800X3D</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$449</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>3.4 GHz</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>4.5 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Core i9-10850K</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$299</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>10-Core</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>3.6 GHz</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>5.2 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Ryzen 5 4600G</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$154</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>3.7 GHz</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>4.2 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Core i7-10700K</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$329</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>3.8 GHz</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>5.10 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Ryzen 5 4500</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$118</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Socket AM4</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>4.1 GHz</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>DNE</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Core i3-12100</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$116</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Quad-Core</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>3.3 GHz</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>P-core Turbo Frequency: Up to 4.30 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Core i7-12700F</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$312</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>12-Core (8P+4E)</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>P-core Base Frequency: 2.1 GHzE-core Base Frequency: 1.6 GHz</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 4.9 GHzP-core Turbo Frequency: Up to 4.8 GHzE-core Turbo Frequency: Up to 3.6 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Core i9-12900KS</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$747</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>16-Core (8P+8E)</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>P-core Base Frequency: 3.4 GHzE-core Base Frequency: 2.5 GHz</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Intel Thermal Velocity Boost Max Frequency: 5.5 GHzIntel Turbo Boost Max Technology 3.0 Frequency: 5.3 GHzPerformance-core Max Turbo Frequency: 5.2 GHzEfficient-core Max Turbo Frequency: 4 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Core i5-11600K</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$209</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>3.9 GHz</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>4.9 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Core i7-11700KF</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$298</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>3.6 GHz</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>5.0 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Core i9-10900</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$379</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>10-Core</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2.8 GHz</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>5.20 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Core i9-10900K</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>$389</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>10-Core</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>3.7 GHz</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>5.30 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Core i7-12700KF</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>$377</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>12-Core (8P+4E)</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Core i5-12600KF</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>$259</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>LGA 1700</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>10-Core (6P+4E)</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>P-core Base Frequency: 3.7 GHzE-core Base Frequency: 2.8 GHz</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Single P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.6 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Core i5-11400F</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>$149</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>6-Core</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2.6 GHz</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>4.4 GHz</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Core i9-11900</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>$319</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>LGA 1200</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>8-Core</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2.5 GHz</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>5.2 GHz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Certain indexes in the final posting have shifted positions. Something in WebFunctions is not appending data properly and needs to be addressed. Investigate indexes 45,52,54,61,63,65. These indexes are where the program appends incorrectly.
Additionally, need to change WebFunctions to remove item from search_list so that when an object is found, it is skipped over in continued searches.

Signed-off-by: Upterry <mattleroy11@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerPartsData.xlsx
+++ b/ComputerPartsData.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,32 +510,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$173</t>
+          <t>$159</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$173</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.5 GHz</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>3.5 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -552,32 +552,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$173</t>
+          <t>$159</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$173</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.5 GHz</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>3.5 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -599,27 +599,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$589</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>16-Core (8P+8E)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>16-Core (8P+8E)</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>P-core Base Frequency: 3.2 GHzE-core Base Frequency: 2.4 GHz</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.2 GHzE-core Base Frequency: 2.4 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.2 GHzSingle P-core Turbo Frequency: Up to 5.1 GHzSingle E-core Turbo Frequency: Up to 3.9 GHz</t>
         </is>
       </c>
     </row>
@@ -641,27 +641,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$199</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.7 GHz</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>4.6 GHz</t>
         </is>
       </c>
     </row>
@@ -678,32 +678,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$319</t>
+          <t>$317</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$319</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: 5.00 GHzIntel Turbo Boost Technology 2.0 Frequency: 4.90 GHz</t>
         </is>
       </c>
     </row>
@@ -720,32 +720,32 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>$269</t>
+          <t>$249</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$269</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>4.6 GHz</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>4.6 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
     </row>
@@ -762,32 +762,32 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$168</t>
+          <t>$161</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>$168</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2.5 GHz</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2.5 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -804,32 +804,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>$409</t>
+          <t>$358</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>$409</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>12-Core</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>12-Core</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>3.7 GHz</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>4.8 GHz</t>
         </is>
       </c>
     </row>
@@ -851,27 +851,27 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>$279</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>10-Core (6P+4E)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>10-Core (6P+4E)</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>P-core Base Frequency: 3.7 GHzE-core Base Frequency: 2.8 GHz</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.7 GHzE-core Base Frequency: 2.8 GHz</t>
+          <t>Single P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.6 GHz</t>
         </is>
       </c>
     </row>
@@ -888,32 +888,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>$139</t>
+          <t>$128</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>$139</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4.2 GHz</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>4.2 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
     </row>
@@ -935,27 +935,27 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>$391</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.5 GHz</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>3.5 GHz</t>
+          <t>Intel Thermal Velocity Boost Frequency: 5.30 GHzIntel Turbo Boost Max Technology 3.0 Frequency: 5.20 GHzIntel Turbo Boost Technology 2.0 Frequency: 5.10 GHz</t>
         </is>
       </c>
     </row>
@@ -972,32 +972,32 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>$319</t>
+          <t>$288</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>$319</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.8 GHz</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>4.7 GHz</t>
         </is>
       </c>
     </row>
@@ -1019,27 +1019,27 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>$399</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>12-Core (8P+4E)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>12-Core (8P+4E)</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
       </c>
     </row>
@@ -1056,32 +1056,32 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>$183</t>
+          <t>$148</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>$183</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.9 GHz</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>3.9 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -1098,32 +1098,32 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$117</t>
+          <t>$118</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>$117</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2.9 GHz</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2.9 GHz</t>
+          <t>4.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1140,32 +1140,32 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>$158</t>
+          <t>$164</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>$158</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>4.2 GHz</t>
         </is>
       </c>
     </row>
@@ -1187,27 +1187,27 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>$109</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3.3 GHz</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>3.3 GHz</t>
+          <t>4.3 GHz</t>
         </is>
       </c>
     </row>
@@ -1224,32 +1224,32 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>$553</t>
+          <t>$503</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>$553</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>16-Core</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>16-Core</t>
+          <t>32</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>3.4 GHz</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>3.4 GHz</t>
+          <t>4.9 GHz</t>
         </is>
       </c>
     </row>
@@ -1266,32 +1266,32 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>$185</t>
+          <t>$182</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>$185</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2.5 GHz</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2.5 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -1308,32 +1308,32 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>$289</t>
+          <t>$249</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>$289</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.8 GHz</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>4.6 GHz</t>
         </is>
       </c>
     </row>
@@ -1355,27 +1355,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>$203</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4.1 GHz</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>4.1 GHz</t>
+          <t>4.80 GHz</t>
         </is>
       </c>
     </row>
@@ -1392,32 +1392,32 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>$449</t>
+          <t>$448</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>$449</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.4 GHz</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>3.4 GHz</t>
+          <t>4.5 GHz</t>
         </is>
       </c>
     </row>
@@ -1439,27 +1439,27 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>$349</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>10-Core</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>10-Core</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>5.2 GHz</t>
         </is>
       </c>
     </row>
@@ -1481,27 +1481,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>$154</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.7 GHz</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>4.2 GHz</t>
         </is>
       </c>
     </row>
@@ -1523,27 +1523,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>$328</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.8 GHz</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>5.10 GHz</t>
         </is>
       </c>
     </row>
@@ -1565,27 +1565,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>$112</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4.1 GHz</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>4.1 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
     </row>
@@ -1607,27 +1607,27 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>$129</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3.3 GHz</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>3.3 GHz</t>
+          <t>P-core Turbo Frequency: Up to 4.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1649,27 +1649,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>$312</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>12-Core (8P+4E)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>12-Core (8P+4E)</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>P-core Base Frequency: 2.1 GHzE-core Base Frequency: 1.6 GHz</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 2.1 GHzE-core Base Frequency: 1.6 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 4.9 GHzP-core Turbo Frequency: Up to 4.8 GHzE-core Turbo Frequency: Up to 3.6 GHz</t>
         </is>
       </c>
     </row>
@@ -1686,32 +1686,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>$749</t>
+          <t>$747</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>$749</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>16-Core (8P+8E)</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>16-Core (8P+8E)</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>P-core Base Frequency: 3.4 GHzE-core Base Frequency: 2.5 GHz</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.4 GHzE-core Base Frequency: 2.5 GHz</t>
+          <t>Intel Thermal Velocity Boost Max Frequency: 5.5 GHzIntel Turbo Boost Max Technology 3.0 Frequency: 5.3 GHzPerformance-core Max Turbo Frequency: 5.2 GHzEfficient-core Max Turbo Frequency: 4 GHz</t>
         </is>
       </c>
     </row>
@@ -1728,32 +1728,32 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>$208</t>
+          <t>$224</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>$208</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.9 GHz</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>3.9 GHz</t>
+          <t>4.9 GHz</t>
         </is>
       </c>
     </row>
@@ -1775,27 +1775,27 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>$298</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>5.0 GHz</t>
         </is>
       </c>
     </row>
@@ -1817,69 +1817,69 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>$379</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>10-Core</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>10-Core</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>2.8 GHz</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2.8 GHz</t>
+          <t>5.20 GHz</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Core i9-10900K</t>
+          <t>Ryzen 5 5600</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>$389</t>
+          <t>$159</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>$389</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>10-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>3.5 GHz</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -1891,37 +1891,37 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Core i7-12700KF</t>
+          <t>Core i9-10900K</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>$377</t>
+          <t>$389</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>$377</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>10-Core</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>12-Core (8P+4E)</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>3.7 GHz</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
+          <t>5.30 GHz</t>
         </is>
       </c>
     </row>
@@ -1933,37 +1933,37 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Core i5-12600KF</t>
+          <t>Core i7-12700KF</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>$249</t>
+          <t>$377</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>$249</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>12-Core (8P+4E)</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>10-Core (6P+4E)</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>P-core Base Frequency: 3.6 GHzE-core Base Frequency: 2.7 GHz</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.7 GHzE-core Base Frequency: 2.8 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.0 GHzSingle P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.8 GHz</t>
         </is>
       </c>
     </row>
@@ -1975,37 +1975,37 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Core i5-11400F</t>
+          <t>Core i5-12600KF</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>$151</t>
+          <t>$259</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>$151</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>10-Core (6P+4E)</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>P-core Base Frequency: 3.7 GHzE-core Base Frequency: 2.8 GHz</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2.6 GHz</t>
+          <t>Single P-core Turbo Frequency: Up to 4.9 GHzSingle E-core Turbo Frequency: Up to 3.6 GHz</t>
         </is>
       </c>
     </row>
@@ -2017,79 +2017,79 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Core i7-10700KF</t>
+          <t>Core i5-11400F</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>$289</t>
+          <t>$149</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>$289</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>2.6 GHz</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ryzen 5 5600</t>
+          <t>Core i7-10700</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>$173</t>
+          <t>$284</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>$173</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2.9 GHz</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>3.5 GHz</t>
+          <t>4.80 GHz</t>
         </is>
       </c>
     </row>
@@ -2101,37 +2101,37 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Core i7-12700</t>
+          <t>Core i7-10700KF</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>$342</t>
+          <t>$289</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>$342</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>12-Core (8P+4E)</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>3.8 GHz</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 2.1 GHzE-core Base Frequency: 1.6 GHz</t>
+          <t>5.10 GHz</t>
         </is>
       </c>
     </row>
@@ -2143,37 +2143,37 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Core i7-11700</t>
+          <t>Core i9-11900</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>$313</t>
+          <t>$319</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>$313</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>2.5 GHz</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2.5 GHz</t>
+          <t>5.2 GHz</t>
         </is>
       </c>
     </row>
@@ -2185,37 +2185,37 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Core i5-10400</t>
+          <t>Core i7-12700</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>$146</t>
+          <t>$342</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>$146</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>12-Core (8P+4E)</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>P-core Base Frequency: 2.1 GHzE-core Base Frequency: 1.6 GHz</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2.9 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 4.9 GHzP-core Turbo Frequency: Up to 4.8 GHzE-core Turbo Frequency: Up to 3.6 GHz</t>
         </is>
       </c>
     </row>
@@ -2227,37 +2227,37 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Core i5-12600</t>
+          <t>Core i7-11700</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>$229</t>
+          <t>$313</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>$229</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2.5 GHz</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>3.3 GHz</t>
+          <t>4.9 GHz</t>
         </is>
       </c>
     </row>
@@ -2269,79 +2269,79 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Core i9-11900KF</t>
+          <t>Core i5-10400</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>$379</t>
+          <t>$146</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>$379</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>2.9 GHz</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>3.5 GHz</t>
+          <t>4.30 GHz</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>Core i5-12600</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>$428</t>
+          <t>$229</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>$428</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2.5 GHz</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>5.2 GHz</t>
+          <t>3.3 GHz</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>P-core Max Turbo Frequency: Up to 4.8 GHz</t>
         </is>
       </c>
     </row>
@@ -2353,79 +2353,79 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Core i7-10700F</t>
+          <t>Core i9-11900KF</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>$DNE</t>
+          <t>$379</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>$DNE</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.5 GHz</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2.9 GHz</t>
+          <t>Intel Thermal Velocity Boost Frequency: 5.30 GHzIntel Turbo Boost Max Technology 3.0 Frequency: 5.20 GHzIntel Turbo Boost Technology 2.0 Frequency: 5.10 GHz</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Core i5-11600KF</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>$209</t>
+          <t>$428</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>$209</t>
+          <t>16</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>2.5 GHz</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>5.2 GHz</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>3.9 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
     </row>
@@ -2437,37 +2437,37 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Core i5-10600KF</t>
+          <t>Core i7-10700F</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>$179</t>
+          <t>$234</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>$179</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2.9 GHz</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>4.1 GHz</t>
+          <t>4.80 GHz</t>
         </is>
       </c>
     </row>
@@ -2479,37 +2479,37 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Core i5-11600</t>
+          <t>Core i5-11600KF</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>$218</t>
+          <t>$209</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>$218</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.9 GHz</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2.8 GHz</t>
+          <t>4.9 GHz</t>
         </is>
       </c>
     </row>
@@ -2521,37 +2521,37 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Core i3-10100</t>
+          <t>Core i5-10600KF</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>$110</t>
+          <t>$179</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>$110</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4.1 GHz</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>4.80 GHz</t>
         </is>
       </c>
     </row>
@@ -2563,79 +2563,79 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Core i9-12900KF</t>
+          <t>Core i5-11600</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>$549</t>
+          <t>$224</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>$549</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>16-Core (8P+8E)</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>2.8 GHz</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>P-core Base Frequency: 3.2 GHzE-core Base Frequency: 2.4 GHz</t>
+          <t>4.8 GHz</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Core i3-10100</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>$110</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>LGA 1200</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>6-Core</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>$219</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>$219</t>
-        </is>
-      </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>3.3 GHz</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>4.80 GHz</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>4.30 GHz</t>
         </is>
       </c>
     </row>
@@ -2647,37 +2647,37 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Core i5-12500</t>
+          <t>Core i9-12900KF</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>$202</t>
+          <t>$549</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>$202</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>LGA 1700</t>
+          <t>16-Core (8P+8E)</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>P-core Base Frequency: 3.2 GHzE-core Base Frequency: 2.4 GHz</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>3.0 GHz</t>
+          <t>Intel Turbo Boost Max Technology 3.0 Frequency: Up to 5.2 GHzSingle P-core Turbo Frequency: Up to 5.1 GHzSingle E-core Turbo Frequency: Up to 3.9 GHz</t>
         </is>
       </c>
     </row>
@@ -2694,27 +2694,27 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>$193</t>
+          <t>$219</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>$193</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.3 GHz</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>3.1 GHz</t>
+          <t>4.80 GHz</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>4.50 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2731,79 +2731,79 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Core i9-10900KF</t>
+          <t>Core i5-12500</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>$359</t>
+          <t>$202</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>$359</t>
+          <t>LGA 1700</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>10-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>3.0 GHz</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>P-core Max Turbo Frequency: Up to 4.6 GHz</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Core i5-11400</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>$172</t>
+          <t>$199</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>$172</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>3.1 GHz</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>4.50 GHz</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2.6 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
     </row>
@@ -2815,37 +2815,37 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Core i7-11700F</t>
+          <t>Core i9-10900KF</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>$288</t>
+          <t>$359</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>$288</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>10-Core</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.7 GHz</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2.5 GHz</t>
+          <t>5.30 GHz</t>
         </is>
       </c>
     </row>
@@ -2857,163 +2857,163 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Core i3-10100F</t>
+          <t>Core i7-11700F</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>$76</t>
+          <t>$288</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>$76</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>LGA 1200</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2.5 GHz</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>4.9 GHz</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Ryzen Threadripper 3970X</t>
+          <t>Core i5-11400</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>$3,198</t>
+          <t>$163</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>$3,198</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Socket sTRX4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>32-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>2.6 GHz</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>Intel Turbo Boost Technology 2.0 Frequency: 4.40 GHz</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Intel</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Ryzen 7 3700X</t>
+          <t>Core i3-10100F</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>$259</t>
+          <t>$76</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>$259</t>
+          <t>LGA 1200</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>Quad-Core</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>4.30 GHz</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Core i7-7700</t>
+          <t>Ryzen 7 3700X</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>$258</t>
+          <t>$246</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>$258</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>LGA 1151</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>4.4 GHz</t>
         </is>
       </c>
     </row>
@@ -3025,200 +3025,200 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Ryzen 7 2700X</t>
+          <t>Ryzen 5 3500X</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>$214</t>
+          <t>$139</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>$214</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>3.7 GHz</t>
+          <t>4.1GHz</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Socket sWRX8</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Ryzen 7 2700</t>
+          <t>32-Core</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>$149</t>
+          <t>$3,374</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>$149</t>
+          <t>64</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>3.5 GHz</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>4.2 GHz</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>3.2 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>$209</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>$209</t>
+          <t>Ryzen Threadripper 3960X</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>$1,532</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>Socket sTRX4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>24-Core</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>48</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>3.8 GHz</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>Up to 4.5 GHz</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Socket sWRX8</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Core i7-4790</t>
+          <t>64-Core</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>$134</t>
+          <t>$7,490</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>$134</t>
+          <t>128</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>LGA 1150</t>
+          <t>2.7 GHz</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Quad-Core</t>
+          <t>4.2 GHz</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>4.0GHz</t>
+          <t>DNE</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>$99</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>$99</t>
+          <t>Athlon 3000G</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>$77</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>Dual-Core</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>DNE</t>
+          <t>3.5 GHz</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -3230,42 +3230,42 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>$99</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Ryzen Threadripper 3960X</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>$1,499</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>$1,499</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Socket sTRX4</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>24-Core</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>DNE</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>DNE</t>
         </is>
       </c>
     </row>
@@ -3277,331 +3277,121 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Ryzen 5 3600X</t>
+          <t>Ryzen 7 2700</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>$209</t>
+          <t>$149</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>$209</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Socket AM4</t>
+          <t>8-Core</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>6-Core</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3.2 GHz</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>3.8 GHz</t>
+          <t>4.1 GHz</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Core i7-9700</t>
+          <t>Ryzen 5 2600X</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>$275</t>
+          <t>$142</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>$275</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>LGA 1151 (300 Series)</t>
+          <t>6-Core</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3.6 GHz</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>3.0 GHz</t>
+          <t>4.2 GHz</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Core i9-9900KF</t>
+          <t>Ryzen 9 3900X</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>$473</t>
+          <t>$476</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>$473</t>
+          <t>Socket AM4</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>LGA 1151 (300 Series)</t>
+          <t>12-Core</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>8-Core</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3.8 GHz</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>3.6 GHz</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>AMD</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Ryzen 7 5800X</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>$307</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>$307</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>Socket AM4</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>8-Core</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>3.8 GHz</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Intel</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Core i7-4790K</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>$202</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>$202</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>LGA 1150</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>Quad-Core</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>4.0 GHz</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>AMD</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Athlon 200GE</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>$70</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>$70</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>Socket AM4</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>Dual-Core</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>3.2 GHz</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Intel</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Celeron G6900</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>$39</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>$39</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>LGA 1700</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Dual-Core</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>3.4 GHz</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>AMD</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Ryzen 5 3500X</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>$149</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>$149</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>Socket AM4</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>6-Core</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>3.6 GHz</t>
+          <t>4.6 GHz</t>
         </is>
       </c>
     </row>

</xml_diff>